<commit_message>
avance 3.0 de software lector de excel
</commit_message>
<xml_diff>
--- a/data/empresas.xlsx
+++ b/data/empresas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\software_mapas_ICA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41F40F7-EBDF-4FE3-8AB4-4B93F66FE3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8829BCA-5D96-48B9-B6D3-333EB54B5841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="790" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FERIAS" sheetId="20" r:id="rId1"/>
@@ -6306,7 +6306,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6908,6 +6908,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -12040,8 +12043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE22"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -14171,8 +14174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y71"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -14249,10 +14252,10 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
-      <c r="S2" s="163" t="s">
+      <c r="S2" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="163"/>
+      <c r="T2" s="176"/>
       <c r="U2" s="162" t="s">
         <v>44</v>
       </c>
@@ -14325,7 +14328,7 @@
         <v>4</v>
       </c>
       <c r="U3" s="106" t="s">
-        <v>5</v>
+        <v>1739</v>
       </c>
       <c r="V3" s="106" t="s">
         <v>6</v>
@@ -19550,10 +19553,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:N2"/>
-    <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="A43:D43">
@@ -20024,8 +20026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -20137,7 +20139,7 @@
         <v>4</v>
       </c>
       <c r="P3" s="106" t="s">
-        <v>5</v>
+        <v>1739</v>
       </c>
       <c r="Q3" s="106" t="s">
         <v>6</v>
@@ -23311,8 +23313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -23430,7 +23432,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="107" t="s">
-        <v>5</v>
+        <v>1739</v>
       </c>
       <c r="N3" s="107" t="s">
         <v>60</v>
@@ -23770,8 +23772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD68"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -28498,8 +28500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="I26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -28606,7 +28608,7 @@
         <v>4</v>
       </c>
       <c r="N3" s="106" t="s">
-        <v>5</v>
+        <v>1739</v>
       </c>
       <c r="O3" s="106" t="s">
         <v>60</v>
@@ -31325,8 +31327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AT19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -31400,9 +31402,7 @@
       <c r="M2" s="162"/>
       <c r="N2" s="162"/>
       <c r="O2" s="162"/>
-      <c r="P2" s="153" t="s">
-        <v>104</v>
-      </c>
+      <c r="P2" s="153"/>
       <c r="Q2" s="162" t="s">
         <v>70</v>
       </c>
@@ -31473,7 +31473,9 @@
       <c r="O3" s="150" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="154"/>
+      <c r="P3" s="154" t="s">
+        <v>104</v>
+      </c>
       <c r="Q3" s="159" t="s">
         <v>105</v>
       </c>

</xml_diff>